<commit_message>
Backup QR Scanner data - 2025-12-10T10:17:34.757Z - Cache Bust: 1765361854757
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Psychiatry_scanner1759398086755_272efcfda7bd3208e090f05a24198cc42a8b7c15230d58e6534a6eec0a74da5a.xlsx
+++ b/log_history/Y4_B2526_Psychiatry_scanner1759398086755_272efcfda7bd3208e090f05a24198cc42a8b7c15230d58e6534a6eec0a74da5a.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Psychiatry" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -433,7 +433,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>12:41:38</v>
+        <v>11:41:38</v>
       </c>
       <c r="E2" t="str">
         <v>Scan</v>
@@ -453,7 +453,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D3" t="str">
-        <v>12:41:44</v>
+        <v>11:41:44</v>
       </c>
       <c r="E3" t="str">
         <v>Scan</v>
@@ -473,7 +473,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D4" t="str">
-        <v>12:41:53</v>
+        <v>11:41:53</v>
       </c>
       <c r="E4" t="str">
         <v>Manual</v>
@@ -493,7 +493,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D5" t="str">
-        <v>12:42:03</v>
+        <v>11:42:03</v>
       </c>
       <c r="E5" t="str">
         <v>Manual</v>
@@ -513,7 +513,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D6" t="str">
-        <v>12:42:08</v>
+        <v>11:42:08</v>
       </c>
       <c r="E6" t="str">
         <v>Scan</v>
@@ -533,7 +533,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D7" t="str">
-        <v>12:42:24</v>
+        <v>11:42:24</v>
       </c>
       <c r="E7" t="str">
         <v>Manual</v>
@@ -553,7 +553,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D8" t="str">
-        <v>12:42:27</v>
+        <v>11:42:27</v>
       </c>
       <c r="E8" t="str">
         <v>Scan</v>
@@ -573,7 +573,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D9" t="str">
-        <v>12:42:34</v>
+        <v>11:42:34</v>
       </c>
       <c r="E9" t="str">
         <v>Manual</v>
@@ -593,7 +593,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D10" t="str">
-        <v>12:42:42</v>
+        <v>11:42:42</v>
       </c>
       <c r="E10" t="str">
         <v>Scan</v>
@@ -613,7 +613,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D11" t="str">
-        <v>12:42:56</v>
+        <v>11:42:56</v>
       </c>
       <c r="E11" t="str">
         <v>Scan</v>
@@ -633,7 +633,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D12" t="str">
-        <v>12:43:07</v>
+        <v>11:43:07</v>
       </c>
       <c r="E12" t="str">
         <v>Manual</v>
@@ -653,7 +653,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D13" t="str">
-        <v>12:43:14</v>
+        <v>11:43:14</v>
       </c>
       <c r="E13" t="str">
         <v>Scan</v>
@@ -673,7 +673,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D14" t="str">
-        <v>12:43:25</v>
+        <v>11:43:25</v>
       </c>
       <c r="E14" t="str">
         <v>Manual</v>
@@ -693,7 +693,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D15" t="str">
-        <v>12:43:32</v>
+        <v>11:43:32</v>
       </c>
       <c r="E15" t="str">
         <v>Manual</v>
@@ -713,7 +713,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D16" t="str">
-        <v>12:43:35</v>
+        <v>11:43:35</v>
       </c>
       <c r="E16" t="str">
         <v>Scan</v>
@@ -733,7 +733,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D17" t="str">
-        <v>12:43:45</v>
+        <v>11:43:45</v>
       </c>
       <c r="E17" t="str">
         <v>Scan</v>
@@ -753,7 +753,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D18" t="str">
-        <v>12:43:50</v>
+        <v>11:43:50</v>
       </c>
       <c r="E18" t="str">
         <v>Scan</v>
@@ -773,7 +773,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>12:43:59</v>
+        <v>11:43:59</v>
       </c>
       <c r="E19" t="str">
         <v>Manual</v>
@@ -793,7 +793,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>12:44:06</v>
+        <v>11:44:06</v>
       </c>
       <c r="E20" t="str">
         <v>Manual</v>
@@ -813,7 +813,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>12:44:09</v>
+        <v>11:44:09</v>
       </c>
       <c r="E21" t="str">
         <v>Scan</v>
@@ -833,7 +833,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>12:44:17</v>
+        <v>11:44:17</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -853,7 +853,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>12:44:23</v>
+        <v>11:44:23</v>
       </c>
       <c r="E23" t="str">
         <v>Scan</v>
@@ -873,7 +873,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>12:44:27</v>
+        <v>11:44:27</v>
       </c>
       <c r="E24" t="str">
         <v>Scan</v>
@@ -893,7 +893,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>12:44:34</v>
+        <v>11:44:34</v>
       </c>
       <c r="E25" t="str">
         <v>Scan</v>
@@ -913,7 +913,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>12:44:42</v>
+        <v>11:44:42</v>
       </c>
       <c r="E26" t="str">
         <v>Scan</v>
@@ -933,7 +933,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>12:44:53</v>
+        <v>11:44:53</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -953,7 +953,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>12:44:58</v>
+        <v>11:44:58</v>
       </c>
       <c r="E28" t="str">
         <v>Scan</v>
@@ -973,7 +973,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>12:45:04</v>
+        <v>11:45:04</v>
       </c>
       <c r="E29" t="str">
         <v>Scan</v>
@@ -993,7 +993,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>12:45:14</v>
+        <v>11:45:14</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1013,7 +1013,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>12:45:20</v>
+        <v>11:45:20</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1033,7 +1033,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>12:45:28</v>
+        <v>11:45:28</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1053,7 +1053,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>12:45:37</v>
+        <v>11:45:37</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1073,7 +1073,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>12:45:43</v>
+        <v>11:45:43</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1093,7 +1093,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>12:46:43</v>
+        <v>11:46:43</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1113,7 +1113,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>12:47:01</v>
+        <v>11:47:01</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1133,7 +1133,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>12:47:07</v>
+        <v>11:47:07</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1153,7 +1153,7 @@
         <v>02/10/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>12:47:12</v>
+        <v>11:47:12</v>
       </c>
       <c r="E38" t="str">
         <v>Scan</v>

</xml_diff>